<commit_message>
Testado com arquivo original do siga
</commit_message>
<xml_diff>
--- a/Base.xlsx
+++ b/Base.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJETOS\NEW_ETIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atentoglobal-my.sharepoint.com/personal/ab995362_br_atento_com/Documents/Documentos/PROJETO/GSIGA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372F0C75-7CBC-47B7-B29F-426356B3638E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{372F0C75-7CBC-47B7-B29F-426356B3638E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1866EFB6-6358-4461-B0C3-B6CAD7B072F0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="3">
-  <si>
-    <t>Demis Souza Silva</t>
-  </si>
-  <si>
-    <t>RE</t>
-  </si>
-  <si>
-    <t>Nome</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
+  <si>
+    <t>RE do usuário</t>
+  </si>
+  <si>
+    <t>Nome usuário</t>
+  </si>
+  <si>
+    <t>Login NT</t>
+  </si>
+  <si>
+    <t>Nº CH vpn</t>
+  </si>
+  <si>
+    <t>Nº CH ramal</t>
+  </si>
+  <si>
+    <t>Nº do ramal</t>
+  </si>
+  <si>
+    <t>Status Field</t>
+  </si>
+  <si>
+    <t>Elisangela da Penha Genezio</t>
+  </si>
+  <si>
+    <t>AB1407782</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRISCILA RODRIGUES DIAMANTINO </t>
+  </si>
+  <si>
+    <t>AB1424227</t>
+  </si>
+  <si>
+    <t>DEBORA DA COSTA NEVES ESPOSITO</t>
+  </si>
+  <si>
+    <t>AB1424158</t>
+  </si>
+  <si>
+    <t>Elizangela Marques de Souza</t>
+  </si>
+  <si>
+    <t>AB1375191</t>
+  </si>
+  <si>
+    <t>MARILAN SANTANA ARAUJO</t>
+  </si>
+  <si>
+    <t>AB1288300</t>
+  </si>
+  <si>
+    <t>EMILY PRATES DA CRUZ</t>
+  </si>
+  <si>
+    <t>AB1301427</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JAQUELINE DA SILVA CALACA BARROS </t>
+  </si>
+  <si>
+    <t>AB1424222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARILIA LIMA DE ALENCAR </t>
+  </si>
+  <si>
+    <t>AB1427466</t>
+  </si>
+  <si>
+    <t>Weverton Vieira Dos Santos Souza</t>
+  </si>
+  <si>
+    <t>AB1424219</t>
+  </si>
+  <si>
+    <t>Samara dos Santos</t>
+  </si>
+  <si>
+    <t>AB1349044</t>
+  </si>
+  <si>
+    <t>KELLY CRISTINA SOUZA DA SILVA</t>
+  </si>
+  <si>
+    <t>ab1427473</t>
+  </si>
+  <si>
+    <t>JAQUELINE DE SOUZA ALMEIDA SEABRA</t>
+  </si>
+  <si>
+    <t>ab1427463</t>
+  </si>
+  <si>
+    <t>MONIQUE CRISTINE DA SILVA  ARAUJO</t>
+  </si>
+  <si>
+    <t>AB1427469</t>
   </si>
 </sst>
 </file>
@@ -351,168 +444,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>995362</v>
+        <v>1407782</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>995362</v>
+        <v>1424227</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>995362</v>
+        <v>1424158</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>995362</v>
+        <v>1375191</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>995362</v>
+        <v>1288300</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>995362</v>
+        <v>1301427</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>995362</v>
+        <v>1424222</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>995362</v>
+        <v>1427466</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>995362</v>
+        <v>1424219</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>995362</v>
+        <v>1349044</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>995362</v>
+        <v>1427473</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>995362</v>
+        <v>1427463</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>995362</v>
+        <v>1427469</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>995362</v>
-      </c>
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>995362</v>
-      </c>
-      <c r="B16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>995362</v>
-      </c>
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>995362</v>
-      </c>
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>995362</v>
-      </c>
-      <c r="B19" t="s">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>